<commit_message>
NoteBook and Conversation Update
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/Character_Data.xlsx
+++ b/GameDesign/ExcelData/Character_Data.xlsx
@@ -5,27 +5,36 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UCSC\GPM\game 271\Project\Nameless_Temp\GameDesign\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-Temp\NamelessHill\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3564F111-E13C-4D4C-AEDA-FB5176ECBAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169EB229-62D8-4DBE-B475-46503C3A307B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2472" yWindow="4932" windowWidth="13752" windowHeight="7428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="54">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,9 +175,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>animName</t>
-  </si>
-  <si>
     <t>突击步枪手</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -209,19 +215,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>iconName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>campName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BtnLRpos</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>campPosIndex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>animPrefab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectIcon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>campIcon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[[0:1001]]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>converIds</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -563,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -579,11 +597,11 @@
     <col min="25" max="25" width="10.6640625" style="1" customWidth="1"/>
     <col min="26" max="26" width="12.6640625" customWidth="1"/>
     <col min="27" max="27" width="14.109375" customWidth="1"/>
-    <col min="28" max="29" width="13.109375" customWidth="1"/>
-    <col min="30" max="30" width="15.44140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="13.109375" customWidth="1"/>
+    <col min="29" max="29" width="15.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -668,8 +686,11 @@
       <c r="AB1" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="AC1" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -740,31 +761,33 @@
         <v>36</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="Y2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="AB2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AD2"/>
+        <v>47</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1">
         <v>200</v>
@@ -827,28 +850,30 @@
         <v>26</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AA3" s="1">
         <v>2</v>
       </c>
       <c r="AB3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD3"/>
+        <v>-1</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1002</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>31</v>
@@ -914,28 +939,30 @@
         <v>26</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AA4" s="1">
         <v>0</v>
       </c>
       <c r="AB4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AD4"/>
+        <v>1</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1003</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -1001,28 +1028,30 @@
         <v>26</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AA5" s="1">
         <v>1</v>
       </c>
       <c r="AB5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="AD5"/>
+        <v>1</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1004</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>33</v>
@@ -1088,23 +1117,25 @@
         <v>26</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Z6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA6" s="1">
         <v>3</v>
       </c>
       <c r="AB6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD6"/>
+        <v>-1</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1005</v>
       </c>
@@ -1175,13 +1206,13 @@
         <v>26</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA7" s="1">
         <v>0</v>
@@ -1189,9 +1220,11 @@
       <c r="AB7" s="1">
         <v>1</v>
       </c>
-      <c r="AD7"/>
+      <c r="AC7" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1006</v>
       </c>
@@ -1262,13 +1295,13 @@
         <v>26</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA8" s="1">
         <v>0</v>
@@ -1276,9 +1309,11 @@
       <c r="AB8" s="1">
         <v>1</v>
       </c>
-      <c r="AD8"/>
+      <c r="AC8" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1007</v>
       </c>
@@ -1349,13 +1384,13 @@
         <v>26</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA9" s="1">
         <v>0</v>
@@ -1363,9 +1398,11 @@
       <c r="AB9" s="1">
         <v>1</v>
       </c>
-      <c r="AD9"/>
+      <c r="AC9" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1008</v>
       </c>
@@ -1436,13 +1473,13 @@
         <v>26</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA10" s="1">
         <v>0</v>
@@ -1450,7 +1487,9 @@
       <c r="AB10" s="1">
         <v>1</v>
       </c>
-      <c r="AD10"/>
+      <c r="AC10" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Unlock Conversation Effect and Unlock Note Effect Update
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/Character_Data.xlsx
+++ b/GameDesign/ExcelData/Character_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-Temp\NamelessHill\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169EB229-62D8-4DBE-B475-46503C3A307B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D552DA-27AB-487D-AE6A-FC331CA1FFCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2472" yWindow="4932" windowWidth="13752" windowHeight="7428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -584,7 +584,7 @@
   <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC7" sqref="AC7"/>
+      <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remake Battle structure update
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/Character_Data.xlsx
+++ b/GameDesign/ExcelData/Character_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-Temp\NamelessHill\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E64D23-D60C-4433-A10B-6B06C7F2BBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE0A7E3-3F79-4C3E-97D9-D38122E1F125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="62">
   <si>
     <t>Id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -269,6 +269,14 @@
   </si>
   <si>
     <t>[[0:1051]]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crAtkSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atkSpeed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -613,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD11"/>
+  <dimension ref="A1:AF11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD3" sqref="AD3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -624,17 +632,19 @@
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="18.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
-    <col min="4" max="22" width="8.88671875" style="1"/>
-    <col min="23" max="23" width="15" style="1" customWidth="1"/>
-    <col min="24" max="25" width="12.109375" customWidth="1"/>
-    <col min="26" max="26" width="10.6640625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="12.6640625" customWidth="1"/>
-    <col min="28" max="28" width="14.109375" customWidth="1"/>
-    <col min="29" max="29" width="13.109375" customWidth="1"/>
-    <col min="30" max="30" width="15.44140625" style="1" customWidth="1"/>
+    <col min="4" max="12" width="8.88671875" style="1"/>
+    <col min="13" max="14" width="14.88671875" style="1" customWidth="1"/>
+    <col min="15" max="24" width="8.88671875" style="1"/>
+    <col min="25" max="25" width="15" style="1" customWidth="1"/>
+    <col min="26" max="27" width="12.109375" customWidth="1"/>
+    <col min="28" max="28" width="10.6640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="12.6640625" customWidth="1"/>
+    <col min="30" max="30" width="14.109375" customWidth="1"/>
+    <col min="31" max="31" width="13.109375" customWidth="1"/>
+    <col min="32" max="32" width="15.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -693,22 +703,22 @@
         <v>20</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="X1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Z1" s="3" t="s">
         <v>19</v>
@@ -717,16 +727,22 @@
         <v>19</v>
       </c>
       <c r="AB1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -764,61 +780,67 @@
         <v>10</v>
       </c>
       <c r="M2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="193.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" ht="193.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1001</v>
       </c>
@@ -856,61 +878,67 @@
         <v>60</v>
       </c>
       <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="O3" s="1">
         <v>2</v>
       </c>
-      <c r="N3" s="1">
+      <c r="P3" s="1">
         <v>5</v>
       </c>
-      <c r="O3" s="1">
+      <c r="Q3" s="1">
         <v>6</v>
       </c>
-      <c r="P3" s="1">
+      <c r="R3" s="1">
         <v>80</v>
       </c>
-      <c r="Q3" s="1">
-        <v>1</v>
-      </c>
-      <c r="R3" s="1">
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
         <v>70</v>
       </c>
-      <c r="S3" s="1">
-        <v>1</v>
-      </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W3" s="1">
+      <c r="X3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y3" s="1">
         <v>0</v>
       </c>
-      <c r="X3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="Z3" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="AA3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AB3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD3" s="1">
         <v>2</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AE3" s="1">
         <v>-1</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="193.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" ht="193.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1002</v>
       </c>
@@ -951,58 +979,64 @@
         <v>1</v>
       </c>
       <c r="N4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1">
         <v>2</v>
       </c>
-      <c r="O4" s="1">
+      <c r="Q4" s="1">
         <v>2</v>
       </c>
-      <c r="P4" s="1">
+      <c r="R4" s="1">
         <v>100</v>
       </c>
-      <c r="Q4" s="1">
-        <v>1</v>
-      </c>
-      <c r="R4" s="1">
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1">
         <v>80</v>
       </c>
-      <c r="S4" s="1">
-        <v>1</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="V4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W4" s="1">
+      <c r="X4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y4" s="1">
         <v>0</v>
       </c>
-      <c r="X4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="Z4" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="AA4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AB4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD4" s="1">
         <v>0</v>
       </c>
-      <c r="AC4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AE4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1003</v>
       </c>
@@ -1043,13 +1077,13 @@
         <v>1</v>
       </c>
       <c r="N5" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O5" s="1">
         <v>1</v>
       </c>
       <c r="P5" s="1">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="Q5" s="1">
         <v>1</v>
@@ -1060,41 +1094,47 @@
       <c r="S5" s="1">
         <v>1</v>
       </c>
-      <c r="T5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U5" s="1" t="s">
+      <c r="T5" s="1">
+        <v>100</v>
+      </c>
+      <c r="U5" s="1">
+        <v>1</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="W5" s="1">
+      <c r="Y5" s="1">
         <v>0</v>
       </c>
-      <c r="X5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="Z5" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="AA5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AB5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="151.80000000000001" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" ht="151.80000000000001" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1004</v>
       </c>
@@ -1135,58 +1175,64 @@
         <v>1</v>
       </c>
       <c r="N6" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O6" s="1">
         <v>1</v>
       </c>
       <c r="P6" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>1</v>
+      </c>
+      <c r="R6" s="1">
         <v>50</v>
       </c>
-      <c r="Q6" s="1">
-        <v>1</v>
-      </c>
-      <c r="R6" s="1">
+      <c r="S6" s="1">
+        <v>1</v>
+      </c>
+      <c r="T6" s="1">
         <v>80</v>
       </c>
-      <c r="S6" s="1">
-        <v>1</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="1">
+        <v>1</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="W6" s="1">
+      <c r="Y6" s="1">
         <v>0</v>
       </c>
-      <c r="X6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="Z6" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="AA6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD6" s="1">
         <v>3</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AE6" s="1">
         <v>-1</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AF6" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1005</v>
       </c>
@@ -1224,61 +1270,67 @@
         <v>100</v>
       </c>
       <c r="M7" s="1">
+        <v>1</v>
+      </c>
+      <c r="N7" s="1">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1">
         <v>0.5</v>
       </c>
-      <c r="N7" s="1">
+      <c r="P7" s="1">
         <v>2</v>
       </c>
-      <c r="O7" s="1">
+      <c r="Q7" s="1">
         <v>2</v>
       </c>
-      <c r="P7" s="1">
+      <c r="R7" s="1">
         <v>90</v>
       </c>
-      <c r="Q7" s="1">
-        <v>1</v>
-      </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
+        <v>1</v>
+      </c>
+      <c r="T7" s="1">
         <v>100</v>
       </c>
-      <c r="S7" s="1">
-        <v>1</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U7" s="1" t="s">
+      <c r="U7" s="1">
+        <v>1</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="V7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W7" s="1">
+      <c r="X7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y7" s="1">
         <v>25</v>
       </c>
-      <c r="X7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="Z7" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="AA7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD7" s="1">
         <v>0</v>
       </c>
-      <c r="AC7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AE7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1006</v>
       </c>
@@ -1316,19 +1368,19 @@
         <v>100</v>
       </c>
       <c r="M8" s="1">
+        <v>1</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1">
         <v>0.5</v>
       </c>
-      <c r="N8" s="1">
+      <c r="P8" s="1">
         <v>2</v>
       </c>
-      <c r="O8" s="1">
+      <c r="Q8" s="1">
         <v>2</v>
-      </c>
-      <c r="P8" s="1">
-        <v>100</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>1</v>
       </c>
       <c r="R8" s="1">
         <v>100</v>
@@ -1336,41 +1388,47 @@
       <c r="S8" s="1">
         <v>1</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>26</v>
+      <c r="T8" s="1">
+        <v>100</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W8" s="1">
+      <c r="W8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y8" s="1">
         <v>10</v>
       </c>
-      <c r="X8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y8" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="Z8" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="AA8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AB8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD8" s="1">
         <v>0</v>
       </c>
-      <c r="AC8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AE8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1007</v>
       </c>
@@ -1408,19 +1466,19 @@
         <v>100</v>
       </c>
       <c r="M9" s="1">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1</v>
+      </c>
+      <c r="O9" s="1">
         <v>0.5</v>
       </c>
-      <c r="N9" s="1">
+      <c r="P9" s="1">
         <v>2</v>
       </c>
-      <c r="O9" s="1">
+      <c r="Q9" s="1">
         <v>2</v>
-      </c>
-      <c r="P9" s="1">
-        <v>100</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>1</v>
       </c>
       <c r="R9" s="1">
         <v>100</v>
@@ -1428,41 +1486,47 @@
       <c r="S9" s="1">
         <v>1</v>
       </c>
-      <c r="T9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>26</v>
+      <c r="T9" s="1">
+        <v>100</v>
+      </c>
+      <c r="U9" s="1">
+        <v>1</v>
       </c>
       <c r="V9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W9" s="1">
+      <c r="W9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y9" s="1">
         <v>10</v>
       </c>
-      <c r="X9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y9" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="Z9" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="AA9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AB9" s="1">
+      <c r="AB9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD9" s="1">
         <v>0</v>
       </c>
-      <c r="AC9" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD9" s="1" t="s">
+      <c r="AE9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1008</v>
       </c>
@@ -1500,19 +1564,19 @@
         <v>100</v>
       </c>
       <c r="M10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1">
         <v>0.5</v>
       </c>
-      <c r="N10" s="1">
+      <c r="P10" s="1">
         <v>2</v>
       </c>
-      <c r="O10" s="1">
+      <c r="Q10" s="1">
         <v>2</v>
-      </c>
-      <c r="P10" s="1">
-        <v>100</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>1</v>
       </c>
       <c r="R10" s="1">
         <v>100</v>
@@ -1520,41 +1584,47 @@
       <c r="S10" s="1">
         <v>1</v>
       </c>
-      <c r="T10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>26</v>
+      <c r="T10" s="1">
+        <v>100</v>
+      </c>
+      <c r="U10" s="1">
+        <v>1</v>
       </c>
       <c r="V10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="W10" s="1">
+      <c r="W10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y10" s="1">
         <v>10</v>
       </c>
-      <c r="X10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="Z10" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="AA10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AB10" s="1">
+      <c r="AB10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD10" s="1">
         <v>0</v>
       </c>
-      <c r="AC10" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="1" t="s">
+      <c r="AE10" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="207" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" ht="207" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1009</v>
       </c>
@@ -1592,57 +1662,63 @@
         <v>60</v>
       </c>
       <c r="M11" s="1">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1">
         <v>2</v>
       </c>
-      <c r="N11" s="1">
+      <c r="P11" s="1">
         <v>4</v>
       </c>
-      <c r="O11" s="1">
+      <c r="Q11" s="1">
         <v>6</v>
       </c>
-      <c r="P11" s="1">
+      <c r="R11" s="1">
         <v>80</v>
       </c>
-      <c r="Q11" s="1">
-        <v>1</v>
-      </c>
-      <c r="R11" s="1">
+      <c r="S11" s="1">
+        <v>1</v>
+      </c>
+      <c r="T11" s="1">
         <v>70</v>
       </c>
-      <c r="S11" s="1">
-        <v>1</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>25</v>
+      <c r="U11" s="1">
+        <v>1</v>
       </c>
       <c r="V11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="W11" s="1">
+      <c r="W11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y11" s="1">
         <v>0</v>
       </c>
-      <c r="X11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y11" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="Z11" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="AA11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AB11" s="1">
+      <c r="AB11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD11" s="1">
         <v>4</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AE11" s="1">
         <v>-1</v>
       </c>
-      <c r="AD11" s="1" t="s">
+      <c r="AF11" s="1" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
battle some fixed update
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/Character_Data.xlsx
+++ b/GameDesign/ExcelData/Character_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-Temp\NamelessHill\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE0A7E3-3F79-4C3E-97D9-D38122E1F125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78BFF45-A7EA-477D-B810-8F54EF79341A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
   <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -632,9 +632,10 @@
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="18.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="1" customWidth="1"/>
-    <col min="4" max="12" width="8.88671875" style="1"/>
-    <col min="13" max="14" width="14.88671875" style="1" customWidth="1"/>
-    <col min="15" max="24" width="8.88671875" style="1"/>
+    <col min="4" max="13" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="14.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="14" style="1" customWidth="1"/>
+    <col min="16" max="24" width="8.88671875" style="1"/>
     <col min="25" max="25" width="15" style="1" customWidth="1"/>
     <col min="26" max="27" width="12.109375" customWidth="1"/>
     <col min="28" max="28" width="10.6640625" style="1" customWidth="1"/>
@@ -780,13 +781,13 @@
         <v>10</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>61</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>12</v>
@@ -878,13 +879,13 @@
         <v>60</v>
       </c>
       <c r="M3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3" s="1">
         <v>0.5</v>
       </c>
       <c r="O3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P3" s="1">
         <v>5</v>
@@ -1270,13 +1271,13 @@
         <v>100</v>
       </c>
       <c r="M7" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N7" s="1">
         <v>1</v>
       </c>
       <c r="O7" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P7" s="1">
         <v>2</v>
@@ -1368,13 +1369,13 @@
         <v>100</v>
       </c>
       <c r="M8" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N8" s="1">
         <v>1</v>
       </c>
       <c r="O8" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P8" s="1">
         <v>2</v>
@@ -1466,13 +1467,13 @@
         <v>100</v>
       </c>
       <c r="M9" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N9" s="1">
         <v>1</v>
       </c>
       <c r="O9" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P9" s="1">
         <v>2</v>
@@ -1564,13 +1565,13 @@
         <v>100</v>
       </c>
       <c r="M10" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N10" s="1">
         <v>1</v>
       </c>
       <c r="O10" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="P10" s="1">
         <v>2</v>
@@ -1662,13 +1663,13 @@
         <v>60</v>
       </c>
       <c r="M11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11" s="1">
         <v>1</v>
       </c>
       <c r="O11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P11" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
test remove pawn completed
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/Character_Data.xlsx
+++ b/GameDesign/ExcelData/Character_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-Temp\NamelessHill\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC8F311-D575-464E-BE74-D26075CEC10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D49F48A-0E53-4CFA-91CF-E3CAE836BA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -661,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P10" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add Name for pawn
</commit_message>
<xml_diff>
--- a/GameDesign/ExcelData/Character_Data.xlsx
+++ b/GameDesign/ExcelData/Character_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NamelessHill\Nameless_Temp\GameDesign\ExcelData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\University\ucsc\GAME 271\project-Nameless Hill\NamelessHill-makeEnd\Nameless_Temp\GameDesign\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BED9FB-5CC9-4101-AD8B-73DE376B1FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96AF19C-B91A-42F2-B487-55BC62E1D2EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="19394" windowHeight="10996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -153,10 +153,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Enemy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>dialogue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -327,6 +323,10 @@
   </si>
   <si>
     <t>Halo, he is the engineer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -682,32 +682,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE8" sqref="AE8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="1"/>
-    <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="18.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="42" style="1" customWidth="1"/>
-    <col min="4" max="13" width="8.875" style="1"/>
-    <col min="14" max="14" width="14.375" style="1" customWidth="1"/>
+    <col min="4" max="13" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="14.33203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="14" style="1" customWidth="1"/>
-    <col min="16" max="23" width="8.875" style="1"/>
-    <col min="24" max="24" width="21.25" style="1" customWidth="1"/>
+    <col min="16" max="23" width="8.88671875" style="1"/>
+    <col min="24" max="24" width="21.21875" style="1" customWidth="1"/>
     <col min="25" max="25" width="15" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.125" customWidth="1"/>
-    <col min="27" max="27" width="16.125" customWidth="1"/>
-    <col min="28" max="28" width="18.75" customWidth="1"/>
-    <col min="29" max="29" width="10.625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="12.625" customWidth="1"/>
-    <col min="31" max="31" width="14.125" customWidth="1"/>
-    <col min="32" max="32" width="13.125" customWidth="1"/>
-    <col min="33" max="33" width="15.5" style="1" customWidth="1"/>
+    <col min="26" max="26" width="12.109375" customWidth="1"/>
+    <col min="27" max="27" width="16.109375" customWidth="1"/>
+    <col min="28" max="28" width="18.77734375" customWidth="1"/>
+    <col min="29" max="29" width="10.6640625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="12.6640625" customWidth="1"/>
+    <col min="31" max="31" width="14.109375" customWidth="1"/>
+    <col min="32" max="32" width="13.109375" customWidth="1"/>
+    <col min="33" max="33" width="15.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -787,7 +787,7 @@
         <v>19</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB1" s="3" t="s">
         <v>19</v>
@@ -808,7 +808,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -849,10 +849,10 @@
         <v>11</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>12</v>
@@ -882,42 +882,42 @@
         <v>29</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AD2" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="AE2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1001</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="1">
         <v>500</v>
@@ -980,7 +980,7 @@
         <v>25</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y3" s="1">
         <v>0</v>
@@ -992,13 +992,13 @@
         <v>1</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AE3" s="1">
         <v>5</v>
@@ -1007,18 +1007,18 @@
         <v>-1</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1002</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1">
         <v>500</v>
@@ -1093,13 +1093,13 @@
         <v>1</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AE4" s="1">
         <v>0</v>
@@ -1108,18 +1108,18 @@
         <v>1</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1003</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="1">
         <v>500</v>
@@ -1182,7 +1182,7 @@
         <v>25</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y5" s="1">
         <v>0</v>
@@ -1194,13 +1194,13 @@
         <v>1</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AD5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AE5" s="1">
         <v>1</v>
@@ -1209,18 +1209,18 @@
         <v>1</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1004</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1">
         <v>500</v>
@@ -1283,7 +1283,7 @@
         <v>28</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Y6" s="1">
         <v>0</v>
@@ -1295,13 +1295,13 @@
         <v>1</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AE6" s="1">
         <v>3</v>
@@ -1310,18 +1310,18 @@
         <v>-1</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1005</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1">
         <v>500</v>
@@ -1384,7 +1384,7 @@
         <v>23</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y7" s="1">
         <v>0</v>
@@ -1396,13 +1396,13 @@
         <v>1</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AE7" s="1">
         <v>4</v>
@@ -1411,18 +1411,18 @@
         <v>-1</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" ht="69" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1006</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1">
         <v>500</v>
@@ -1497,13 +1497,13 @@
         <v>1</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AE8" s="1">
         <v>2</v>
@@ -1512,18 +1512,18 @@
         <v>-1</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1007</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="1">
         <v>100</v>
@@ -1598,13 +1598,13 @@
         <v>1</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AE9" s="1">
         <v>0</v>
@@ -1616,15 +1616,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1008</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="1">
         <v>100</v>
@@ -1699,13 +1699,13 @@
         <v>1</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AE10" s="1">
         <v>0</v>
@@ -1717,12 +1717,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1009</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>31</v>
@@ -1800,13 +1800,13 @@
         <v>1</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AE11" s="1">
         <v>0</v>
@@ -1818,12 +1818,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1010</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>31</v>
@@ -1901,13 +1901,13 @@
         <v>1</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AE12" s="1">
         <v>0</v>
@@ -1919,15 +1919,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>1011</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>32</v>
+      <c r="B13" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="6">
         <v>100</v>
@@ -2002,13 +2002,13 @@
         <v>0</v>
       </c>
       <c r="AB13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AC13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AD13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AE13" s="6">
         <v>0</v>

</xml_diff>